<commit_message>
Restructure tables and fixtures in evaluation section. Removed unnecessary information, replaced placeholder info in some diagrams.
</commit_message>
<xml_diff>
--- a/data/processed/classification-expset-1/tables.xlsx
+++ b/data/processed/classification-expset-1/tables.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25711"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atyndall/Dropbox/ash-honours/thesis/data/processed/classification-expset-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\ash-honours\thesis\data\processed\classification-expset-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="33200" windowHeight="20520" tabRatio="500"/>
+    <workbookView xWindow="156" yWindow="456" windowWidth="33204" windowHeight="20520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="59">
   <si>
     <t>ZeroR</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Relation Incl</t>
   </si>
   <si>
-    <t>Nominal Balanced</t>
-  </si>
-  <si>
     <t>K*</t>
   </si>
   <si>
@@ -191,13 +188,19 @@
     <t>Incl. 0</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>$R^2$</t>
-  </si>
-  <si>
     <t>IBK Num</t>
+  </si>
+  <si>
+    <t>$r$</t>
+  </si>
+  <si>
+    <t>KNN (Numeric)$^1$</t>
+  </si>
+  <si>
+    <t>KNN (Nominal)$^1$</t>
+  </si>
+  <si>
+    <t>\%</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,6 +467,9 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="181">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -653,6 +659,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -921,28 +930,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="3" width="22.1640625" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" customWidth="1"/>
-    <col min="12" max="12" width="23.1640625" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="22.19921875" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" customWidth="1"/>
+    <col min="11" max="11" width="20.796875" customWidth="1"/>
+    <col min="12" max="12" width="23.19921875" customWidth="1"/>
+    <col min="13" max="13" width="15.19921875" customWidth="1"/>
+    <col min="14" max="14" width="16.69921875" customWidth="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1"/>
+    <col min="16" max="16" width="17.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="D2">
         <v>1</v>
       </c>
@@ -971,12 +982,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="C3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1019,7 +1030,7 @@
       </c>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1062,7 +1073,7 @@
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1070,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1">
         <v>0.30499999999999999</v>
@@ -1105,7 +1116,7 @@
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1159,7 @@
       </c>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1202,7 @@
       </c>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1245,7 @@
       </c>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="C10" t="s">
         <v>29</v>
       </c>
@@ -1250,7 +1261,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1293,7 +1304,7 @@
       </c>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1347,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1344,7 +1355,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1">
         <v>0.2555</v>
@@ -1379,7 +1390,7 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1422,7 +1433,7 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1465,7 +1476,7 @@
       </c>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1508,7 +1519,7 @@
       </c>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -1551,12 +1562,13 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1587,23 +1599,11 @@
       <c r="L20" t="s">
         <v>49</v>
       </c>
-      <c r="M20" t="s">
-        <v>33</v>
-      </c>
-      <c r="N20" t="s">
-        <v>35</v>
-      </c>
-      <c r="P20" t="s">
-        <v>55</v>
-      </c>
-      <c r="R20" t="s">
-        <v>56</v>
-      </c>
       <c r="T20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1622,32 +1622,26 @@
       <c r="F21">
         <v>0.79100000000000004</v>
       </c>
+      <c r="M21" t="s">
+        <v>33</v>
+      </c>
       <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P21" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21" t="s">
+        <v>52</v>
+      </c>
+      <c r="U21" t="s">
         <v>53</v>
       </c>
-      <c r="O21" t="s">
-        <v>54</v>
-      </c>
-      <c r="P21" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>54</v>
-      </c>
-      <c r="R21" t="s">
-        <v>53</v>
-      </c>
-      <c r="S21" t="s">
-        <v>54</v>
-      </c>
-      <c r="T21" t="s">
-        <v>53</v>
-      </c>
-      <c r="U21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1670,7 +1664,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1696,19 +1690,20 @@
         <v>42</v>
       </c>
       <c r="M23" t="s">
-        <v>21</v>
-      </c>
-      <c r="O23" s="1">
-        <v>0.36430000000000001</v>
-      </c>
-      <c r="Q23" s="6">
+        <v>56</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="O23" s="6">
         <v>65.649600000000007</v>
       </c>
+      <c r="Q23" s="6"/>
       <c r="T23" s="1">
         <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1728,16 +1723,19 @@
         <v>0.70599999999999996</v>
       </c>
       <c r="J24" t="s">
-        <v>57</v>
-      </c>
-      <c r="O24">
-        <v>1.1234999999999999</v>
-      </c>
-      <c r="S24">
-        <v>0.37659999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="M24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.59209999999999996</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0.68710000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1763,16 +1761,16 @@
         <v>40</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="N25" s="1">
-        <v>0.59209999999999996</v>
-      </c>
-      <c r="R25" s="1">
-        <v>0.68710000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.5252</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.5887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1798,16 +1796,16 @@
         <v>41</v>
       </c>
       <c r="M26" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0.5252</v>
-      </c>
-      <c r="R26" s="1">
-        <v>0.5887</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="N26">
+        <v>1.123</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0.37659999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1827,10 +1825,10 @@
         <v>0.26</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1856,20 +1854,15 @@
         <v>42</v>
       </c>
       <c r="M28" t="s">
-        <v>22</v>
-      </c>
-      <c r="N28" s="1">
-        <v>0.2888</v>
-      </c>
-      <c r="O28" s="1">
-        <v>0.2898</v>
-      </c>
-      <c r="P28" s="6">
-        <v>84.957300000000004</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>77.559100000000001</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="P28" s="5">
+        <v>0.75960000000000005</v>
+      </c>
+      <c r="Q28" s="6"/>
       <c r="T28" s="1">
         <v>0.85</v>
       </c>
@@ -1877,7 +1870,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1903,20 +1896,15 @@
         <v>42</v>
       </c>
       <c r="M29" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="N29" s="1">
-        <v>0.29559999999999997</v>
-      </c>
-      <c r="O29" s="1">
-        <v>0.29320000000000002</v>
-      </c>
-      <c r="P29" s="6">
-        <v>84.273499999999999</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>78.248000000000005</v>
-      </c>
+        <v>0.65069999999999995</v>
+      </c>
+      <c r="P29" s="1">
+        <v>-0.11840000000000001</v>
+      </c>
+      <c r="Q29" s="6"/>
       <c r="T29" s="1">
         <v>0.84199999999999997</v>
       </c>
@@ -1924,7 +1912,7 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1949,21 +1937,10 @@
       <c r="L30" t="s">
         <v>42</v>
       </c>
-      <c r="M30" t="s">
-        <v>23</v>
-      </c>
-      <c r="N30" s="1">
-        <v>0.35870000000000002</v>
-      </c>
-      <c r="O30" s="1">
-        <v>0.31969999999999998</v>
-      </c>
-      <c r="P30" s="6">
-        <v>70.857100000000003</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>72.131100000000004</v>
-      </c>
+      <c r="M30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q30" s="6"/>
       <c r="T30" s="1">
         <v>0.70599999999999996</v>
       </c>
@@ -1971,7 +1948,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1997,20 +1974,15 @@
         <v>42</v>
       </c>
       <c r="M31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N31" s="1">
-        <v>0.4093</v>
-      </c>
-      <c r="O31" s="1">
-        <v>0.36780000000000002</v>
-      </c>
-      <c r="P31" s="6">
-        <v>63.7607</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>61.515700000000002</v>
-      </c>
+        <v>0.31380000000000002</v>
+      </c>
+      <c r="O31" s="6">
+        <v>82.393199999999993</v>
+      </c>
+      <c r="Q31" s="6"/>
       <c r="T31" s="1">
         <v>0.625</v>
       </c>
@@ -2018,7 +1990,7 @@
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2044,20 +2016,15 @@
         <v>42</v>
       </c>
       <c r="M32" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="N32" s="1">
-        <v>0.4098</v>
-      </c>
-      <c r="O32" s="1">
-        <v>0.38550000000000001</v>
-      </c>
-      <c r="P32" s="6">
-        <v>65.982900000000001</v>
-      </c>
-      <c r="Q32" s="6">
-        <v>56.889800000000001</v>
-      </c>
+        <v>0.30420000000000003</v>
+      </c>
+      <c r="O32" s="6">
+        <v>82.564099999999996</v>
+      </c>
+      <c r="Q32" s="6"/>
       <c r="T32" s="1">
         <v>0.62</v>
       </c>
@@ -2065,7 +2032,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21">
       <c r="J33" t="s">
         <v>14</v>
       </c>
@@ -2076,20 +2043,15 @@
         <v>42</v>
       </c>
       <c r="M33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N33" s="1">
-        <v>0.47139999999999999</v>
-      </c>
-      <c r="O33" s="1">
-        <v>0.433</v>
-      </c>
-      <c r="P33" s="6">
-        <v>32.4786</v>
-      </c>
-      <c r="Q33" s="6">
-        <v>24.606300000000001</v>
-      </c>
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="O33" s="6">
+        <v>77.142899999999997</v>
+      </c>
+      <c r="Q33" s="6"/>
       <c r="T33" s="1">
         <v>0.26</v>
       </c>
@@ -2097,7 +2059,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2119,11 +2081,17 @@
       <c r="G34" t="s">
         <v>38</v>
       </c>
-      <c r="M34" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0.40529999999999999</v>
+      </c>
+      <c r="O34" s="6">
+        <v>63.589700000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2152,22 +2120,17 @@
         <v>43</v>
       </c>
       <c r="M35" t="s">
-        <v>51</v>
-      </c>
-      <c r="N35" s="5">
-        <v>0.42320000000000002</v>
-      </c>
-      <c r="O35" s="1">
-        <v>0.54959999999999998</v>
-      </c>
-      <c r="R35" s="5">
-        <v>0.75960000000000005</v>
-      </c>
-      <c r="S35" s="1">
-        <v>0.82799999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="O35" s="6">
+        <v>67.179500000000004</v>
+      </c>
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2199,19 +2162,14 @@
         <v>26</v>
       </c>
       <c r="N36" s="1">
-        <v>0.65069999999999995</v>
-      </c>
-      <c r="O36" s="1">
-        <v>0.97189999999999999</v>
-      </c>
-      <c r="R36" s="1">
-        <v>-0.11840000000000001</v>
-      </c>
-      <c r="S36" s="1">
-        <v>-0.1293</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+        <v>0.442</v>
+      </c>
+      <c r="O36" s="6">
+        <v>49.743600000000001</v>
+      </c>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -2230,11 +2188,8 @@
       <c r="F37">
         <v>0.78200000000000003</v>
       </c>
-      <c r="M37" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2262,21 +2217,7 @@
       <c r="L38" t="s">
         <v>45</v>
       </c>
-      <c r="M38" t="s">
-        <v>22</v>
-      </c>
-      <c r="N38" s="1">
-        <v>0.31380000000000002</v>
-      </c>
-      <c r="O38" s="1">
-        <v>0.2878</v>
-      </c>
-      <c r="P38" s="6">
-        <v>82.393199999999993</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>82.907700000000006</v>
-      </c>
+      <c r="Q38" s="6"/>
       <c r="T38" s="7">
         <v>0.81899999999999995</v>
       </c>
@@ -2284,7 +2225,7 @@
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2312,21 +2253,7 @@
       <c r="L39" t="s">
         <v>45</v>
       </c>
-      <c r="M39" t="s">
-        <v>51</v>
-      </c>
-      <c r="N39" s="1">
-        <v>0.30420000000000003</v>
-      </c>
-      <c r="O39" s="1">
-        <v>0.2853</v>
-      </c>
-      <c r="P39" s="6">
-        <v>82.564099999999996</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>82.613</v>
-      </c>
+      <c r="Q39" s="6"/>
       <c r="T39" s="7">
         <v>0.81399999999999995</v>
       </c>
@@ -2334,7 +2261,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2362,21 +2289,7 @@
       <c r="L40" t="s">
         <v>45</v>
       </c>
-      <c r="M40" t="s">
-        <v>23</v>
-      </c>
-      <c r="N40" s="1">
-        <v>0.36209999999999998</v>
-      </c>
-      <c r="O40" s="1">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="P40" s="6">
-        <v>77.142899999999997</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>78.688500000000005</v>
-      </c>
+      <c r="Q40" s="6"/>
       <c r="T40" s="7">
         <v>0.75700000000000001</v>
       </c>
@@ -2384,7 +2297,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2412,21 +2325,7 @@
       <c r="L41" t="s">
         <v>45</v>
       </c>
-      <c r="M41" t="s">
-        <v>24</v>
-      </c>
-      <c r="N41" s="1">
-        <v>0.40529999999999999</v>
-      </c>
-      <c r="O41" s="1">
-        <v>0.35160000000000002</v>
-      </c>
-      <c r="P41" s="6">
-        <v>63.589700000000001</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>66.208299999999994</v>
-      </c>
+      <c r="Q41" s="6"/>
       <c r="T41" s="7">
         <v>0.63200000000000001</v>
       </c>
@@ -2434,7 +2333,7 @@
         <v>0.64400000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2459,21 +2358,7 @@
       <c r="L42" t="s">
         <v>45</v>
       </c>
-      <c r="M42" t="s">
-        <v>25</v>
-      </c>
-      <c r="N42" s="1">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="O42" s="1">
-        <v>0.3795</v>
-      </c>
-      <c r="P42" s="6">
-        <v>67.179500000000004</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>57.465600000000002</v>
-      </c>
+      <c r="Q42" s="6"/>
       <c r="T42" s="7">
         <v>0.64</v>
       </c>
@@ -2481,7 +2366,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2506,21 +2391,7 @@
       <c r="L43" t="s">
         <v>45</v>
       </c>
-      <c r="M43" t="s">
-        <v>26</v>
-      </c>
-      <c r="N43" s="1">
-        <v>0.442</v>
-      </c>
-      <c r="O43" s="1">
-        <v>0.41539999999999999</v>
-      </c>
-      <c r="P43" s="6">
-        <v>49.743600000000001</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>40.3733</v>
-      </c>
+      <c r="Q43" s="6"/>
       <c r="T43" s="7">
         <v>0.33</v>
       </c>
@@ -2528,7 +2399,7 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -2545,7 +2416,7 @@
         <v>0.73409999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2562,7 +2433,7 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -2578,8 +2449,17 @@
       <c r="G46">
         <v>-0.1293</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O46" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>53</v>
+      </c>
+      <c r="S46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -2601,8 +2481,14 @@
       <c r="G48" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O48" s="1">
+        <v>0.36430000000000001</v>
+      </c>
+      <c r="Q48" s="6">
+        <v>65.649600000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2621,8 +2507,14 @@
       <c r="F49">
         <v>0.57399999999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <v>1.1234999999999999</v>
+      </c>
+      <c r="S49">
+        <v>0.37659999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -2642,7 +2534,7 @@
         <v>0.82399999999999995</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2662,7 +2554,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -2682,7 +2574,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2701,8 +2593,14 @@
       <c r="F53">
         <v>0.64400000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O53" s="1">
+        <v>0.2898</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>77.559100000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2721,8 +2619,14 @@
       <c r="F54">
         <v>0.55400000000000005</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O54" s="1">
+        <v>0.29320000000000002</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>78.248000000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -2741,8 +2645,22 @@
       <c r="F55">
         <v>0.23200000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O55" s="1">
+        <v>0.31969999999999998</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>72.131100000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
+      <c r="O56" s="1">
+        <v>0.36780000000000002</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>61.515700000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>32</v>
       </c>
@@ -2764,8 +2682,14 @@
       <c r="G57" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O57" s="1">
+        <v>0.38550000000000001</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>56.889800000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2784,8 +2708,14 @@
       <c r="F58">
         <v>0.82399999999999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O58" s="1">
+        <v>0.433</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>24.606300000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2735,7 @@
         <v>0.81899999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -2824,8 +2754,14 @@
       <c r="F60">
         <v>0.81399999999999995</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O60" s="1">
+        <v>0.54959999999999998</v>
+      </c>
+      <c r="S60" s="1">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -2844,8 +2780,14 @@
       <c r="F61">
         <v>0.75700000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O61" s="1">
+        <v>0.97189999999999999</v>
+      </c>
+      <c r="S61" s="1">
+        <v>-0.1293</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -2865,7 +2807,7 @@
         <v>0.63200000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -2884,8 +2826,14 @@
       <c r="F63">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="O63" s="1">
+        <v>0.2878</v>
+      </c>
+      <c r="Q63" s="6">
+        <v>82.907700000000006</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -2903,6 +2851,44 @@
       </c>
       <c r="F64">
         <v>0.33</v>
+      </c>
+      <c r="O64" s="1">
+        <v>0.2853</v>
+      </c>
+      <c r="Q64" s="6">
+        <v>82.613</v>
+      </c>
+    </row>
+    <row r="65" spans="15:17">
+      <c r="O65" s="1">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="Q65" s="6">
+        <v>78.688500000000005</v>
+      </c>
+    </row>
+    <row r="66" spans="15:17">
+      <c r="O66" s="1">
+        <v>0.35160000000000002</v>
+      </c>
+      <c r="Q66" s="6">
+        <v>66.208299999999994</v>
+      </c>
+    </row>
+    <row r="67" spans="15:17">
+      <c r="O67" s="1">
+        <v>0.3795</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>57.465600000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="15:17">
+      <c r="O68" s="1">
+        <v>0.41539999999999999</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>40.3733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perform significantly more analysis into classification features and enegy efficiency. Generate appropriate tables and plots.
</commit_message>
<xml_diff>
--- a/data/processed/classification-expset-1/tables.xlsx
+++ b/data/processed/classification-expset-1/tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="58">
   <si>
     <t>ZeroR</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>K*</t>
-  </si>
-  <si>
-    <t>Nominal Unbalanced</t>
   </si>
   <si>
     <t>Excl. 0</t>
@@ -932,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1689,10 +1686,10 @@
         <v>35</v>
       </c>
       <c r="O24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -1715,7 +1712,7 @@
         <v>0.625</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -1738,7 +1735,7 @@
         <v>0.62</v>
       </c>
       <c r="M26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N26">
         <v>0.34599999999999997</v>
@@ -1799,10 +1796,10 @@
         <v>0.94499999999999995</v>
       </c>
       <c r="T28" t="s">
+        <v>51</v>
+      </c>
+      <c r="U28" t="s">
         <v>52</v>
-      </c>
-      <c r="U28" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
@@ -1848,7 +1845,7 @@
         <v>42</v>
       </c>
       <c r="M30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N30" s="1">
         <v>0.36399999999999999</v>
@@ -1878,7 +1875,7 @@
         <v>0.68710000000000004</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M31" t="s">
         <v>23</v>
@@ -1930,7 +1927,7 @@
         <v>41</v>
       </c>
       <c r="M33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N33">
         <v>1.123</v>
@@ -2084,7 +2081,7 @@
         <v>42</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="Q37" s="6"/>
       <c r="T37" s="1">
@@ -2601,13 +2598,13 @@
         <v>0.64400000000000002</v>
       </c>
       <c r="O53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>